<commit_message>
Fixed blankPassword_Test and invalidEmail_Test from LoginPageTest class
</commit_message>
<xml_diff>
--- a/src/main/java/testData/InvalidEmails.xlsx
+++ b/src/main/java/testData/InvalidEmails.xlsx
@@ -19,12 +19,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>invalidMail</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>plainaddress</t>
@@ -407,7 +404,7 @@
   <dimension ref="A1:A19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A19"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -420,94 +417,89 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished writing the remaining tests for RecoverPassPageTest
</commit_message>
<xml_diff>
--- a/src/main/java/testData/InvalidEmails.xlsx
+++ b/src/main/java/testData/InvalidEmails.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>invalidMail</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>this\ is"really"not\allowed@example.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -417,6 +420,11 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+    </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
Updated the InvalidEmails excell with a whitespace value
</commit_message>
<xml_diff>
--- a/src/main/java/testData/InvalidEmails.xlsx
+++ b/src/main/java/testData/InvalidEmails.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>invalidMail</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>this\ is"really"not\allowed@example.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    </t>
   </si>
 </sst>
 </file>
@@ -401,110 +404,115 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A18"/>
+  <dimension ref="A1:A19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.5546875" customWidth="1"/>
+    <col min="1" max="1" width="33.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1"/>
+    <hyperlink ref="A4" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>